<commit_message>
the excel files with the driving and transit std dev
</commit_message>
<xml_diff>
--- a/driving_times.xlsx
+++ b/driving_times.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meiaalsup/dev/mit/IDS.131/proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F42B8401-A294-2442-B821-9484F97C32D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8924E93C-7729-A347-B448-2CBCADDD9CA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="driving_times" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">driving_times!$G$2:$G$201</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">driving_times!$G$2:$G$201</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">driving_times!$G$2:$G$201</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -60,9 +58,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -543,7 +541,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1590,11 +1588,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J202"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="J211" sqref="J211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8073,6 +8071,48 @@
         <v>578.39499999999998</v>
       </c>
     </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A203" s="1">
+        <f>STDEV(A2:A201)</f>
+        <v>104.6810379127589</v>
+      </c>
+      <c r="B203" s="1">
+        <f t="shared" ref="B203:J203" si="1">STDEV(B2:B201)</f>
+        <v>113.80936089856905</v>
+      </c>
+      <c r="C203" s="1">
+        <f t="shared" si="1"/>
+        <v>119.69344049902013</v>
+      </c>
+      <c r="D203" s="1">
+        <f t="shared" si="1"/>
+        <v>65.169468874365052</v>
+      </c>
+      <c r="E203" s="1">
+        <f t="shared" si="1"/>
+        <v>134.61862415672368</v>
+      </c>
+      <c r="F203" s="1">
+        <f t="shared" si="1"/>
+        <v>88.805289239914785</v>
+      </c>
+      <c r="G203" s="1">
+        <f t="shared" si="1"/>
+        <v>65.182664865706229</v>
+      </c>
+      <c r="H203" s="1">
+        <f t="shared" si="1"/>
+        <v>98.751429478871884</v>
+      </c>
+      <c r="I203" s="1">
+        <f t="shared" si="1"/>
+        <v>124.93979967453743</v>
+      </c>
+      <c r="J203" s="1">
+        <f t="shared" si="1"/>
+        <v>82.548898102212462</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>